<commit_message>
tests de création de distributions
</commit_message>
<xml_diff>
--- a/quantitative/quant_tool.xlsx
+++ b/quantitative/quant_tool.xlsx
@@ -4,18 +4,50 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>type of scale</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
+    <t>number of bins</t>
+  </si>
+  <si>
+    <t>bins</t>
+  </si>
+  <si>
+    <t>Values (low)</t>
+  </si>
+  <si>
+    <t>scales</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -69,7 +101,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +146,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +181,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +363,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f>IF(F$8&lt;$B$3,F$8+1,"")</f>
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ref="H8:Y8" si="0">IF(G$8&lt;$B$3,G$8+1,"")</f>
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="R8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="T8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="U8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="V8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="W8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="X8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Y8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <f>$B$1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="choose a linear or a log scale" sqref="B4">
+      <formula1>$A$20:$A$21</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>